<commit_message>
quitando lectura en ejecucion y dejando base de datos externa
</commit_message>
<xml_diff>
--- a/Practica 3/Akinnator carros.xlsx
+++ b/Practica 3/Akinnator carros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhon_\OneDrive\Documentos\ing\7° Semestre\Sistemas expertos\2 P\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E38F498-2C24-4C85-B934-E703B665A5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C53364-BD93-4B00-BEB8-E31D6B475F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F407C848-B6E0-4D8C-BB93-A027D34AB3E3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="46">
   <si>
     <t>Nivel 1</t>
   </si>
@@ -53,36 +53,15 @@
     <t>Nivel 5</t>
   </si>
   <si>
-    <t>Toyota Supra Japones 2JZ-GTE I6 TT</t>
-  </si>
-  <si>
     <t>Chevrolet Camaro USA ZL1 LT4 V8 TT</t>
   </si>
   <si>
     <t>Volkswagen Beetle Aleman Boxer4 TT</t>
   </si>
   <si>
-    <t>Nissan Skyline GTR Japones R34 RB26DETT L6 TA</t>
-  </si>
-  <si>
-    <t>Porsche 911 Gt3 RS Aleman Boxer6 TT</t>
-  </si>
-  <si>
-    <t>Ford F-150 Raptor USA Ecoboost V6 T4</t>
-  </si>
-  <si>
     <t>Ford Mustang GT USA Coyote V8 TT</t>
   </si>
   <si>
-    <t>McLaren F1 Britanico V12 TT</t>
-  </si>
-  <si>
-    <t>Lamborghini Murcielago Italiano V12 TA</t>
-  </si>
-  <si>
-    <t>Lamborghini Gallardo Italiano V10 TA</t>
-  </si>
-  <si>
     <t>Ferrari F-40 Italiano V8 TT</t>
   </si>
   <si>
@@ -95,54 +74,21 @@
     <t>Ford Fiesta USA I4 TD</t>
   </si>
   <si>
-    <t>Ford Focus RS USA Ecoboost I4 TA</t>
-  </si>
-  <si>
     <t>Volkswagen Jetta Aleman I4 TD</t>
   </si>
   <si>
     <t>Dodge Charger R/T 1970 USA Hemi V8 TT</t>
   </si>
   <si>
-    <t>Mitsubishi Lancer Evolution 9 Japones I4 TA</t>
-  </si>
-  <si>
-    <t>Subaru Impreza STI Japones Boxer4 TA</t>
-  </si>
-  <si>
-    <t>Chevrolet Impala SS 1994 USA V6 TT</t>
-  </si>
-  <si>
-    <t>Acura NSX Japones V6 TA</t>
-  </si>
-  <si>
-    <t>Bugatti Chiron SS Frances W16 TA</t>
-  </si>
-  <si>
     <t>Chevrolet Astra USA I4 TD</t>
   </si>
   <si>
-    <t>Toyota Corolla 86 Japones I4 TT</t>
-  </si>
-  <si>
-    <t>Lamborghini Aventador J Italiano V12 TA</t>
-  </si>
-  <si>
-    <t>Ferrari La Ferrari Italiano V12 TT</t>
-  </si>
-  <si>
     <t>Mazda 3 Japones Sckyactiv G I4 TD</t>
   </si>
   <si>
     <t>BMW M3 E30 Aleman M20 I6 TT</t>
   </si>
   <si>
-    <t>Mazda Miata Mx-5 Japones Skyactiv G I4 TT</t>
-  </si>
-  <si>
-    <t>Shelby AC Cobra USA 427 V8 TT</t>
-  </si>
-  <si>
     <t>Chevrolet Corvette C6 Z06 USA LT4 V8 TT</t>
   </si>
   <si>
@@ -159,21 +105,6 @@
   </si>
   <si>
     <t>¿Es Traccion Delantera?</t>
-  </si>
-  <si>
-    <t>Lista Completa</t>
-  </si>
-  <si>
-    <t>Lista de TA</t>
-  </si>
-  <si>
-    <t>Lista de TD</t>
-  </si>
-  <si>
-    <t>Lista de TT</t>
-  </si>
-  <si>
-    <t>Lista T4</t>
   </si>
   <si>
     <t>¿Es Estado Unidense?</t>
@@ -633,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC20ECD2-35D9-4C47-B71B-96B8D5D9FD13}">
-  <dimension ref="A1:AG56"/>
+  <dimension ref="A1:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5:AG5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -717,10 +648,10 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -738,7 +669,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -761,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -779,7 +710,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
@@ -799,10 +730,10 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -812,7 +743,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -822,7 +753,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -832,7 +763,7 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -847,7 +778,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -857,7 +788,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -867,7 +798,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -877,7 +808,7 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
@@ -889,52 +820,52 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
@@ -945,37 +876,37 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
@@ -991,70 +922,70 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="U8" s="2"/>
       <c r="V8" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="W8" s="2"/>
       <c r="X8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AG8" s="2"/>
     </row>
@@ -1063,47 +994,47 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="U9" s="2"/>
       <c r="V9" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="W9" s="2"/>
       <c r="X9" s="2" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
@@ -1117,168 +1048,168 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="S11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="W11" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
@@ -1289,284 +1220,117 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B54" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B56" s="1" t="s">
-        <v>36</v>
-      </c>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="Z5:AG5"/>
+    <mergeCell ref="R5:Y5"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="AF9:AG9"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="AD7:AG7"/>
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="J5:Q5"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J7:M7"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="B5:I5"/>
@@ -1583,51 +1347,6 @@
     <mergeCell ref="B3:Q3"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J5:Q5"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="Z9:AA9"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="AF9:AG9"/>
-    <mergeCell ref="AF8:AG8"/>
-    <mergeCell ref="AD7:AG7"/>
-    <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="AD9:AE9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="R3:AG3"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="Z6:AC6"/>
-    <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="Z5:AG5"/>
-    <mergeCell ref="R5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>